<commit_message>
minor changes in sql-ddl-generator
</commit_message>
<xml_diff>
--- a/sql-ddl-generator/google_sheet_excel.xlsx
+++ b/sql-ddl-generator/google_sheet_excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="!@#%^&amp;(($%" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="table 1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="table 2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="table 3" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="61">
   <si>
     <t>merchant_id</t>
   </si>
@@ -153,6 +153,9 @@
     <t>m36</t>
   </si>
   <si>
+    <t>date_values</t>
+  </si>
+  <si>
     <t>fse_id</t>
   </si>
   <si>
@@ -160,21 +163,6 @@
   </si>
   <si>
     <t>fse_score</t>
-  </si>
-  <si>
-    <t>fse1</t>
-  </si>
-  <si>
-    <t>fse2</t>
-  </si>
-  <si>
-    <t>fse3</t>
-  </si>
-  <si>
-    <t>fse4</t>
-  </si>
-  <si>
-    <t>fse5</t>
   </si>
   <si>
     <t>m_state</t>
@@ -193,6 +181,21 @@
   </si>
   <si>
     <t>threshold_higher</t>
+  </si>
+  <si>
+    <t>fse1</t>
+  </si>
+  <si>
+    <t>fse2</t>
+  </si>
+  <si>
+    <t>fse3</t>
+  </si>
+  <si>
+    <t>fse4</t>
+  </si>
+  <si>
+    <t>fse5</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -262,6 +265,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -28950,105 +28962,132 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1.0</v>
-      </c>
+      <c r="A2" s="6">
+        <v>44562.0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2.0</v>
-      </c>
+      <c r="A3" s="6">
+        <v>44563.0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="A4" s="6">
+        <v>44564.0</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1">
-        <v>10.0</v>
-      </c>
+      <c r="A5" s="6">
+        <v>44569.0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1">
-        <v>15.0</v>
+      <c r="A6" s="6">
+        <v>44570.0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <v>44571.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <v>44572.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <v>44573.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>44619.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6">
+        <v>44620.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4">
+        <v>44621.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4">
+        <v>44622.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4">
+        <v>44924.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7">
+        <v>44925.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7">
+        <v>44926.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7">
+        <v>44927.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7">
+        <v>44928.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4">
+        <v>44955.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7">
+        <v>44956.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7">
+        <v>44957.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7">
+        <v>44958.0</v>
       </c>
     </row>
   </sheetData>
@@ -29068,10 +29107,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -29080,7 +29119,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -29092,30 +29131,30 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -29156,10 +29195,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -29200,10 +29239,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -29244,10 +29283,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -29288,10 +29327,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -29332,10 +29371,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -29376,10 +29415,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -29420,10 +29459,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -29464,10 +29503,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -29508,10 +29547,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -29552,10 +29591,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -29596,10 +29635,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -29640,10 +29679,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -29684,10 +29723,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -29728,10 +29767,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -29772,10 +29811,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
@@ -29816,10 +29855,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>23</v>
@@ -29860,10 +29899,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
@@ -29904,10 +29943,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -29948,10 +29987,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>23</v>
@@ -29992,10 +30031,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>23</v>
@@ -30036,10 +30075,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>23</v>
@@ -30080,10 +30119,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>23</v>
@@ -30124,10 +30163,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>23</v>
@@ -30168,10 +30207,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>23</v>

</xml_diff>